<commit_message>
New script for GDPR
Added new script for GDPR verification
</commit_message>
<xml_diff>
--- a/Data files/SSL_scan_data.xlsx
+++ b/Data files/SSL_scan_data.xlsx
@@ -52,7 +52,7 @@
     <t>R3</t>
   </si>
   <si>
-    <t>Not https/no auto-redirect to https</t>
+    <t>No https/no auto-redirect to https</t>
   </si>
   <si>
     <t>cactusglobal.com</t>
@@ -453,7 +453,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>